<commit_message>
Final fix to handle queries that are not in given set
</commit_message>
<xml_diff>
--- a/FinalOutput/Outputs.xlsx
+++ b/FinalOutput/Outputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LongBeach\Sem2-Summer\SearchEngineProject\FinalOutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B12B1BE-095B-4377-BE78-EB06224933B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205997D8-AB2B-4736-8D29-178E7833EA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{6F81E54F-3A14-4A44-9231-98C560F0213D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6F81E54F-3A14-4A44-9231-98C560F0213D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -409,28 +409,28 @@
     <t>Mean average precision : 0.29623590481996237</t>
   </si>
   <si>
-    <t>Mean response time:  0.21016081762240887</t>
-  </si>
-  <si>
-    <t>Average throughput for 1 iterations with 225 queries is:  4.758260894267537</t>
-  </si>
-  <si>
-    <t>Mean response time:  0.1973096743930378</t>
-  </si>
-  <si>
-    <t>Average throughput for 1 iterations with 225 queries is:  5.068175207709357</t>
-  </si>
-  <si>
-    <t>Mean response time:  0.18298162874037402</t>
-  </si>
-  <si>
-    <t>Average throughput for 1 iterations with 225 queries is:  5.46502950533282</t>
-  </si>
-  <si>
-    <t>Mean response time:  0.19500573408671684</t>
-  </si>
-  <si>
-    <t>Average throughput for 1 iterations with 225 queries is:  5.128054334829515</t>
+    <t>Mean response time:  0.203246806987524</t>
+  </si>
+  <si>
+    <t>Average throughput for 1 iterations with 225 queries is:  4.920126494589327</t>
+  </si>
+  <si>
+    <t>Mean response time:  0.15345342860623223</t>
+  </si>
+  <si>
+    <t>Average throughput for 1 iterations with 225 queries is:  6.516635106055798</t>
+  </si>
+  <si>
+    <t>Mean response time:  0.18235452790707504</t>
+  </si>
+  <si>
+    <t>Average throughput for 1 iterations with 225 queries is:  5.483823250660296</t>
+  </si>
+  <si>
+    <t>Mean response time:  0.17086823238049492</t>
+  </si>
+  <si>
+    <t>Average throughput for 1 iterations with 225 queries is:  5.852462953869433</t>
   </si>
 </sst>
 </file>
@@ -836,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DF74C2-C2BA-4E99-B551-8085A633F035}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -890,7 +890,7 @@
         <v>0.26854959763963898</v>
       </c>
       <c r="C3" s="1">
-        <v>7.5473816396496902</v>
+        <v>7.7713859437522101</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -899,7 +899,7 @@
         <v>0.26898414429148998</v>
       </c>
       <c r="G3" s="1">
-        <v>7.3638914469824899</v>
+        <v>7.55012453779457</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -1406,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C3012B-B153-42A9-90B7-81C800C2BD31}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>